<commit_message>
completed 4/5 excel macro chart Son task
</commit_message>
<xml_diff>
--- a/Test 1.xlsx
+++ b/Test 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="EOL" sheetId="4" r:id="rId3"/>
     <sheet name="Normal_Duration" sheetId="5" r:id="rId4"/>
     <sheet name="EOL_Duration" sheetId="6" r:id="rId5"/>
-    <sheet name="Graph" sheetId="7" r:id="rId6"/>
+    <sheet name="Graph" sheetId="133" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All!$A$1:$E$17</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="59">
   <si>
     <t>AR</t>
   </si>
@@ -205,30 +205,6 @@
   </si>
   <si>
     <t>Pending</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>Aug</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Orages</t>
-  </si>
-  <si>
-    <t>Apples</t>
-  </si>
-  <si>
-    <t>Lemons</t>
   </si>
 </sst>
 </file>
@@ -368,7 +344,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>AR sdfsdf</a:t>
+              <a:t>AR Duration In Design Phase</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -376,83 +352,497 @@
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v/>
+            <c:strRef>
+              <c:f>Graph!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF6600"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-24E7-4073-9BE3-158A9060FFF7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF6600"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-24E7-4073-9BE3-158A9060FFF7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>179</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>227</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>3687</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Pending</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-24E7-4073-9BE3-158A9060FFF7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Graph!$B$1:$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+            <c:numRef>
+              <c:f>Graph!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>Jun</c:v>
+                  <c:v>34094</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>July</c:v>
+                  <c:v>34381</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Aug</c:v>
+                  <c:v>34523</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Sep</c:v>
+                  <c:v>35817</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Oct</c:v>
+                  <c:v>36270</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:pt idx="5">
+                  <c:v>36442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36503</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36508</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36520</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36692</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36728</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36884</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37079</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Graph!$B$2:$F$2</c:f>
+              <c:f>Graph!$B$2:$O$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>130</c:v>
+                <c:pt idx="6">
+                  <c:v>3687</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0E75-4343-9769-F8887502D6B4}"/>
+              <c16:uniqueId val="{00000002-24E7-4073-9BE3-158A9060FFF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -465,57 +855,44 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="158208016"/>
-        <c:axId val="347346208"/>
-        <c:axId val="150865008"/>
-      </c:bar3DChart>
+        <c:axId val="435099840"/>
+        <c:axId val="425771744"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="158208016"/>
+        <c:axId val="435099840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="425771744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="425771744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347346208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="347346208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158208016"/>
+        <c:crossAx val="435099840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:serAx>
-        <c:axId val="150865008"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347346208"/>
-      </c:serAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -533,23 +910,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="44" name="Chart 43">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C08B4A0-498B-4A38-8993-B7CEFA7CE6A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D032FD2-8F05-42B3-BA60-295D540B592D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,8 +1939,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,10 +2184,14 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="10"/>
-      <c r="F8"/>
+      <c r="F8" s="11">
+        <v>39312</v>
+      </c>
       <c r="G8"/>
       <c r="H8"/>
-      <c r="I8"/>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -1856,7 +2237,9 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10"/>
-      <c r="I10"/>
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -2064,90 +2447,69 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:F4"/>
+  <sheetPr codeName="Sheet132"/>
+  <dimension ref="B1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>34094</v>
+      </c>
+      <c r="C1">
+        <v>34381</v>
+      </c>
+      <c r="D1">
+        <v>34523</v>
+      </c>
+      <c r="E1">
+        <v>35817</v>
+      </c>
+      <c r="F1">
+        <v>36270</v>
+      </c>
+      <c r="G1">
+        <v>36442</v>
+      </c>
+      <c r="H1">
+        <v>36503</v>
+      </c>
+      <c r="I1">
+        <v>36508</v>
+      </c>
+      <c r="J1">
+        <v>36520</v>
+      </c>
+      <c r="K1">
+        <v>36692</v>
+      </c>
+      <c r="L1">
+        <v>36728</v>
+      </c>
+      <c r="M1">
+        <v>36798</v>
+      </c>
+      <c r="N1">
+        <v>36884</v>
+      </c>
+      <c r="O1">
+        <v>37079</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>100</v>
+        <v>179</v>
       </c>
       <c r="C2">
-        <v>120</v>
-      </c>
-      <c r="D2">
-        <v>130</v>
-      </c>
-      <c r="E2">
-        <v>105</v>
-      </c>
-      <c r="F2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3">
-        <v>210</v>
-      </c>
-      <c r="C3">
-        <v>230</v>
-      </c>
-      <c r="D3">
-        <v>225</v>
-      </c>
-      <c r="E3">
-        <v>190</v>
-      </c>
-      <c r="F3">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4">
-        <v>150</v>
-      </c>
-      <c r="C4">
-        <v>140</v>
-      </c>
-      <c r="D4">
-        <v>180</v>
-      </c>
-      <c r="E4">
-        <v>150</v>
-      </c>
-      <c r="F4">
-        <v>135</v>
+        <v>227</v>
+      </c>
+      <c r="H2">
+        <v>3687</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
send email to Son
</commit_message>
<xml_diff>
--- a/Test 1.xlsx
+++ b/Test 1.xlsx
@@ -12,7 +12,7 @@
     <sheet name="EOL" sheetId="4" r:id="rId3"/>
     <sheet name="Normal_Duration" sheetId="5" r:id="rId4"/>
     <sheet name="EOL_Duration" sheetId="6" r:id="rId5"/>
-    <sheet name="Graph" sheetId="133" r:id="rId6"/>
+    <sheet name="Graph" sheetId="149" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All!$A$1:$E$17</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="73">
   <si>
     <t>AR</t>
   </si>
@@ -205,6 +205,62 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>34094
+LOCO driver</t>
+  </si>
+  <si>
+    <t>34381
+SCSI board</t>
+  </si>
+  <si>
+    <t>34523
+Prism driver</t>
+  </si>
+  <si>
+    <t>35817
+FCB board KIT</t>
+  </si>
+  <si>
+    <t>36270
+LCD KIT</t>
+  </si>
+  <si>
+    <t>36442
+Copper PT</t>
+  </si>
+  <si>
+    <t>36503
+Keyence TX cable</t>
+  </si>
+  <si>
+    <t>36508
+Keyence R cable</t>
+  </si>
+  <si>
+    <t>36520
+UPS</t>
+  </si>
+  <si>
+    <t>36692
+AT PS</t>
+  </si>
+  <si>
+    <t>36728
+Contactor</t>
+  </si>
+  <si>
+    <t>36798
+750A 5V PS</t>
+  </si>
+  <si>
+    <t>36884
+Fan mounting assy</t>
+  </si>
+  <si>
+    <t>37079
+SAC driver</t>
   </si>
 </sst>
 </file>
@@ -278,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -301,6 +357,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,7 +440,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-24E7-4073-9BE3-158A9060FFF7}"/>
+                <c16:uniqueId val="{00000008-D19F-491D-A87E-2143DEF1BA8D}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -396,7 +455,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-24E7-4073-9BE3-158A9060FFF7}"/>
+                <c16:uniqueId val="{0000000A-D19F-491D-A87E-2143DEF1BA8D}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -424,7 +483,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000002-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -451,7 +510,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000003-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -475,7 +534,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000004-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -499,7 +558,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000005-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -523,7 +582,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000006-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -547,7 +606,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000007-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -574,7 +633,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000008-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -598,7 +657,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{00000009-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -625,7 +684,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{0000000A-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -649,7 +708,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{0000000B-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -673,7 +732,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{0000000C-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -697,7 +756,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{0000000D-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -721,7 +780,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{0000000E-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -745,7 +804,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000010-24E7-4073-9BE3-158A9060FFF7}"/>
+                  <c16:uniqueId val="{0000000F-D19F-491D-A87E-2143DEF1BA8D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -769,55 +828,68 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Graph!$B$1:$O$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>34094</c:v>
+                  <c:v>34094
+LOCO driver</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34381</c:v>
+                  <c:v>34381
+SCSI board</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34523</c:v>
+                  <c:v>34523
+Prism driver</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35817</c:v>
+                  <c:v>35817
+FCB board KIT</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36270</c:v>
+                  <c:v>36270
+LCD KIT</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36442</c:v>
+                  <c:v>36442
+Copper PT</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36503</c:v>
+                  <c:v>36503
+Keyence TX cable</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36508</c:v>
+                  <c:v>36508
+Keyence R cable</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36520</c:v>
+                  <c:v>36520
+UPS</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36692</c:v>
+                  <c:v>36692
+AT PS</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36728</c:v>
+                  <c:v>36728
+Contactor</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36798</c:v>
+                  <c:v>36798
+750A 5V PS</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36884</c:v>
+                  <c:v>36884
+Fan mounting assy</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37079</c:v>
+                  <c:v>37079
+SAC driver</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -842,7 +914,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-24E7-4073-9BE3-158A9060FFF7}"/>
+              <c16:uniqueId val="{00000001-D19F-491D-A87E-2143DEF1BA8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -855,11 +927,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="435099840"/>
-        <c:axId val="425771744"/>
+        <c:axId val="156829712"/>
+        <c:axId val="255994416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="435099840"/>
+        <c:axId val="156829712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,16 +941,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425771744"/>
+        <c:crossAx val="255994416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
+        <c:lblAlgn val="r"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425771744"/>
+        <c:axId val="255994416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +961,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="435099840"/>
+        <c:crossAx val="156829712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -926,7 +998,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D032FD2-8F05-42B3-BA60-295D540B592D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89EB1FFC-87E8-4524-9C8B-3CC90F866706}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2447,55 +2519,55 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet132"/>
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="B1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>34094</v>
-      </c>
-      <c r="C1">
-        <v>34381</v>
-      </c>
-      <c r="D1">
-        <v>34523</v>
-      </c>
-      <c r="E1">
-        <v>35817</v>
-      </c>
-      <c r="F1">
-        <v>36270</v>
-      </c>
-      <c r="G1">
-        <v>36442</v>
-      </c>
-      <c r="H1">
-        <v>36503</v>
-      </c>
-      <c r="I1">
-        <v>36508</v>
-      </c>
-      <c r="J1">
-        <v>36520</v>
-      </c>
-      <c r="K1">
-        <v>36692</v>
-      </c>
-      <c r="L1">
-        <v>36728</v>
-      </c>
-      <c r="M1">
-        <v>36798</v>
-      </c>
-      <c r="N1">
-        <v>36884</v>
-      </c>
-      <c r="O1">
-        <v>37079</v>
+    <row r="1" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>